<commit_message>
refactor code and update base template
</commit_message>
<xml_diff>
--- a/storage/Vexe_Template.xlsx
+++ b/storage/Vexe_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\cvibe-test\storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8976D8C6-0AAC-4CBF-B695-B50CBA0D3DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99E20CC-9B04-462B-87E4-B947AEB1B5C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1639" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1643" uniqueCount="12">
   <si>
     <t>VÉ GỬI XE</t>
   </si>
@@ -13556,8 +13556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
-      <selection activeCell="H213" sqref="H213"/>
+    <sheetView tabSelected="1" topLeftCell="A682" workbookViewId="0">
+      <selection activeCell="D226" sqref="D226:E226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -15433,19 +15433,21 @@
       </c>
       <c r="H153" s="12"/>
     </row>
-    <row r="154" spans="1:8" ht="19.5" customHeight="1">
+    <row r="154" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A154" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B154" s="14"/>
-      <c r="D154" s="13"/>
+      <c r="D154" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="E154" s="14"/>
       <c r="G154" s="13" t="s">
         <v>11</v>
       </c>
       <c r="H154" s="14"/>
     </row>
-    <row r="155" spans="1:8" ht="4.5" customHeight="1"/>
+    <row r="155" spans="1:8" ht="4.5" customHeight="1" thickBot="1"/>
     <row r="156" spans="1:8" ht="15.75" customHeight="1">
       <c r="A156" s="2"/>
       <c r="B156" s="3"/>
@@ -15867,19 +15869,21 @@
       </c>
       <c r="H189" s="12"/>
     </row>
-    <row r="190" spans="1:8" ht="19.5" customHeight="1">
+    <row r="190" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A190" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B190" s="14"/>
-      <c r="D190" s="13"/>
+      <c r="D190" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="E190" s="14"/>
       <c r="G190" s="13" t="s">
         <v>11</v>
       </c>
       <c r="H190" s="14"/>
     </row>
-    <row r="191" spans="1:8" ht="4.5" customHeight="1"/>
+    <row r="191" spans="1:8" ht="4.5" customHeight="1" thickBot="1"/>
     <row r="192" spans="1:8" ht="15.75" customHeight="1">
       <c r="A192" s="2"/>
       <c r="B192" s="3"/>
@@ -16305,19 +16309,21 @@
       </c>
       <c r="H225" s="12"/>
     </row>
-    <row r="226" spans="1:8" ht="19.5" customHeight="1">
+    <row r="226" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A226" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B226" s="14"/>
-      <c r="D226" s="13"/>
+      <c r="D226" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="E226" s="14"/>
       <c r="G226" s="13" t="s">
         <v>11</v>
       </c>
       <c r="H226" s="14"/>
     </row>
-    <row r="227" spans="1:8" ht="4.5" customHeight="1"/>
+    <row r="227" spans="1:8" ht="4.5" customHeight="1" thickBot="1"/>
     <row r="228" spans="1:8" ht="15.75" customHeight="1">
       <c r="A228" s="2"/>
       <c r="B228" s="3"/>
@@ -16739,19 +16745,21 @@
       </c>
       <c r="H261" s="12"/>
     </row>
-    <row r="262" spans="1:8" ht="19.5" customHeight="1">
+    <row r="262" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A262" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B262" s="14"/>
-      <c r="D262" s="13"/>
+      <c r="D262" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="E262" s="14"/>
       <c r="G262" s="13" t="s">
         <v>11</v>
       </c>
       <c r="H262" s="14"/>
     </row>
-    <row r="263" spans="1:8" ht="4.5" customHeight="1"/>
+    <row r="263" spans="1:8" ht="4.5" customHeight="1" thickBot="1"/>
     <row r="264" spans="1:8" ht="15.75" customHeight="1">
       <c r="A264" s="2"/>
       <c r="B264" s="3"/>
@@ -22485,132 +22493,324 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="468">
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="G64:H64"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="G82:H82"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="G76:H76"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="G94:H94"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="G85:H85"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="G91:H91"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="G109:H109"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="G100:H100"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="G103:H103"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="D121:E121"/>
-    <mergeCell ref="G121:H121"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="G112:H112"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="D118:E118"/>
-    <mergeCell ref="G118:H118"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="D136:E136"/>
-    <mergeCell ref="G136:H136"/>
-    <mergeCell ref="A127:B127"/>
-    <mergeCell ref="D127:E127"/>
-    <mergeCell ref="G127:H127"/>
-    <mergeCell ref="A130:B130"/>
-    <mergeCell ref="D130:E130"/>
-    <mergeCell ref="G130:H130"/>
-    <mergeCell ref="A136:B136"/>
-    <mergeCell ref="D244:E244"/>
-    <mergeCell ref="G244:H244"/>
-    <mergeCell ref="A235:B235"/>
-    <mergeCell ref="D235:E235"/>
-    <mergeCell ref="G235:H235"/>
-    <mergeCell ref="A238:B238"/>
-    <mergeCell ref="D238:E238"/>
-    <mergeCell ref="G238:H238"/>
-    <mergeCell ref="A244:B244"/>
-    <mergeCell ref="D256:E256"/>
-    <mergeCell ref="G256:H256"/>
-    <mergeCell ref="A247:B247"/>
-    <mergeCell ref="D247:E247"/>
-    <mergeCell ref="G247:H247"/>
-    <mergeCell ref="A253:B253"/>
-    <mergeCell ref="D253:E253"/>
-    <mergeCell ref="G253:H253"/>
-    <mergeCell ref="A256:B256"/>
-    <mergeCell ref="D271:E271"/>
-    <mergeCell ref="G271:H271"/>
-    <mergeCell ref="A262:B262"/>
-    <mergeCell ref="D262:E262"/>
-    <mergeCell ref="G262:H262"/>
-    <mergeCell ref="A265:B265"/>
-    <mergeCell ref="D265:E265"/>
-    <mergeCell ref="G265:H265"/>
-    <mergeCell ref="A271:B271"/>
-    <mergeCell ref="D283:E283"/>
-    <mergeCell ref="G283:H283"/>
-    <mergeCell ref="A274:B274"/>
-    <mergeCell ref="D274:E274"/>
-    <mergeCell ref="G274:H274"/>
-    <mergeCell ref="A280:B280"/>
-    <mergeCell ref="D280:E280"/>
-    <mergeCell ref="G280:H280"/>
-    <mergeCell ref="A283:B283"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A703:B703"/>
+    <mergeCell ref="D703:E703"/>
+    <mergeCell ref="G703:H703"/>
+    <mergeCell ref="A688:B688"/>
+    <mergeCell ref="D688:E688"/>
+    <mergeCell ref="G688:H688"/>
+    <mergeCell ref="A694:B694"/>
+    <mergeCell ref="D694:E694"/>
+    <mergeCell ref="G694:H694"/>
+    <mergeCell ref="A697:B697"/>
+    <mergeCell ref="D697:E697"/>
+    <mergeCell ref="G697:H697"/>
+    <mergeCell ref="A676:B676"/>
+    <mergeCell ref="D676:E676"/>
+    <mergeCell ref="G676:H676"/>
+    <mergeCell ref="A679:B679"/>
+    <mergeCell ref="D679:E679"/>
+    <mergeCell ref="G679:H679"/>
+    <mergeCell ref="A685:B685"/>
+    <mergeCell ref="D685:E685"/>
+    <mergeCell ref="G685:H685"/>
+    <mergeCell ref="A661:B661"/>
+    <mergeCell ref="D661:E661"/>
+    <mergeCell ref="G661:H661"/>
+    <mergeCell ref="A667:B667"/>
+    <mergeCell ref="D667:E667"/>
+    <mergeCell ref="G667:H667"/>
+    <mergeCell ref="A670:B670"/>
+    <mergeCell ref="D670:E670"/>
+    <mergeCell ref="G670:H670"/>
+    <mergeCell ref="A649:B649"/>
+    <mergeCell ref="D649:E649"/>
+    <mergeCell ref="G649:H649"/>
+    <mergeCell ref="A652:B652"/>
+    <mergeCell ref="D652:E652"/>
+    <mergeCell ref="G652:H652"/>
+    <mergeCell ref="A658:B658"/>
+    <mergeCell ref="D658:E658"/>
+    <mergeCell ref="G658:H658"/>
+    <mergeCell ref="A634:B634"/>
+    <mergeCell ref="D634:E634"/>
+    <mergeCell ref="G634:H634"/>
+    <mergeCell ref="A640:B640"/>
+    <mergeCell ref="D640:E640"/>
+    <mergeCell ref="G640:H640"/>
+    <mergeCell ref="A643:B643"/>
+    <mergeCell ref="D643:E643"/>
+    <mergeCell ref="G643:H643"/>
+    <mergeCell ref="A622:B622"/>
+    <mergeCell ref="D622:E622"/>
+    <mergeCell ref="G622:H622"/>
+    <mergeCell ref="A625:B625"/>
+    <mergeCell ref="D625:E625"/>
+    <mergeCell ref="G625:H625"/>
+    <mergeCell ref="A631:B631"/>
+    <mergeCell ref="D631:E631"/>
+    <mergeCell ref="G631:H631"/>
+    <mergeCell ref="A607:B607"/>
+    <mergeCell ref="D607:E607"/>
+    <mergeCell ref="G607:H607"/>
+    <mergeCell ref="A613:B613"/>
+    <mergeCell ref="D613:E613"/>
+    <mergeCell ref="G613:H613"/>
+    <mergeCell ref="A616:B616"/>
+    <mergeCell ref="D616:E616"/>
+    <mergeCell ref="G616:H616"/>
+    <mergeCell ref="A595:B595"/>
+    <mergeCell ref="D595:E595"/>
+    <mergeCell ref="G595:H595"/>
+    <mergeCell ref="A598:B598"/>
+    <mergeCell ref="D598:E598"/>
+    <mergeCell ref="G598:H598"/>
+    <mergeCell ref="A604:B604"/>
+    <mergeCell ref="D604:E604"/>
+    <mergeCell ref="G604:H604"/>
+    <mergeCell ref="A580:B580"/>
+    <mergeCell ref="D580:E580"/>
+    <mergeCell ref="G580:H580"/>
+    <mergeCell ref="A586:B586"/>
+    <mergeCell ref="D586:E586"/>
+    <mergeCell ref="G586:H586"/>
+    <mergeCell ref="A589:B589"/>
+    <mergeCell ref="D589:E589"/>
+    <mergeCell ref="G589:H589"/>
+    <mergeCell ref="A568:B568"/>
+    <mergeCell ref="D568:E568"/>
+    <mergeCell ref="G568:H568"/>
+    <mergeCell ref="A571:B571"/>
+    <mergeCell ref="D571:E571"/>
+    <mergeCell ref="G571:H571"/>
+    <mergeCell ref="A577:B577"/>
+    <mergeCell ref="D577:E577"/>
+    <mergeCell ref="G577:H577"/>
+    <mergeCell ref="A553:B553"/>
+    <mergeCell ref="D553:E553"/>
+    <mergeCell ref="G553:H553"/>
+    <mergeCell ref="A559:B559"/>
+    <mergeCell ref="D559:E559"/>
+    <mergeCell ref="G559:H559"/>
+    <mergeCell ref="A562:B562"/>
+    <mergeCell ref="D562:E562"/>
+    <mergeCell ref="G562:H562"/>
+    <mergeCell ref="A541:B541"/>
+    <mergeCell ref="D541:E541"/>
+    <mergeCell ref="G541:H541"/>
+    <mergeCell ref="A544:B544"/>
+    <mergeCell ref="D544:E544"/>
+    <mergeCell ref="G544:H544"/>
+    <mergeCell ref="A550:B550"/>
+    <mergeCell ref="D550:E550"/>
+    <mergeCell ref="G550:H550"/>
+    <mergeCell ref="A526:B526"/>
+    <mergeCell ref="D526:E526"/>
+    <mergeCell ref="G526:H526"/>
+    <mergeCell ref="A532:B532"/>
+    <mergeCell ref="D532:E532"/>
+    <mergeCell ref="G532:H532"/>
+    <mergeCell ref="A535:B535"/>
+    <mergeCell ref="D535:E535"/>
+    <mergeCell ref="G535:H535"/>
+    <mergeCell ref="A514:B514"/>
+    <mergeCell ref="D514:E514"/>
+    <mergeCell ref="G514:H514"/>
+    <mergeCell ref="A517:B517"/>
+    <mergeCell ref="D517:E517"/>
+    <mergeCell ref="G517:H517"/>
+    <mergeCell ref="A523:B523"/>
+    <mergeCell ref="D523:E523"/>
+    <mergeCell ref="G523:H523"/>
+    <mergeCell ref="A499:B499"/>
+    <mergeCell ref="D499:E499"/>
+    <mergeCell ref="G499:H499"/>
+    <mergeCell ref="A505:B505"/>
+    <mergeCell ref="D505:E505"/>
+    <mergeCell ref="G505:H505"/>
+    <mergeCell ref="A508:B508"/>
+    <mergeCell ref="D508:E508"/>
+    <mergeCell ref="G508:H508"/>
+    <mergeCell ref="A487:B487"/>
+    <mergeCell ref="D487:E487"/>
+    <mergeCell ref="G487:H487"/>
+    <mergeCell ref="A490:B490"/>
+    <mergeCell ref="D490:E490"/>
+    <mergeCell ref="G490:H490"/>
+    <mergeCell ref="A496:B496"/>
+    <mergeCell ref="D496:E496"/>
+    <mergeCell ref="G496:H496"/>
+    <mergeCell ref="A472:B472"/>
+    <mergeCell ref="D472:E472"/>
+    <mergeCell ref="G472:H472"/>
+    <mergeCell ref="A478:B478"/>
+    <mergeCell ref="D478:E478"/>
+    <mergeCell ref="G478:H478"/>
+    <mergeCell ref="A481:B481"/>
+    <mergeCell ref="D481:E481"/>
+    <mergeCell ref="G481:H481"/>
+    <mergeCell ref="A463:B463"/>
+    <mergeCell ref="D463:E463"/>
+    <mergeCell ref="G463:H463"/>
+    <mergeCell ref="A469:B469"/>
+    <mergeCell ref="D469:E469"/>
+    <mergeCell ref="G469:H469"/>
+    <mergeCell ref="A454:B454"/>
+    <mergeCell ref="D454:E454"/>
+    <mergeCell ref="G454:H454"/>
+    <mergeCell ref="A460:B460"/>
+    <mergeCell ref="D460:E460"/>
+    <mergeCell ref="G460:H460"/>
+    <mergeCell ref="A442:B442"/>
+    <mergeCell ref="D442:E442"/>
+    <mergeCell ref="G442:H442"/>
+    <mergeCell ref="A445:B445"/>
+    <mergeCell ref="D445:E445"/>
+    <mergeCell ref="G445:H445"/>
+    <mergeCell ref="A451:B451"/>
+    <mergeCell ref="D451:E451"/>
+    <mergeCell ref="G451:H451"/>
+    <mergeCell ref="A427:B427"/>
+    <mergeCell ref="D427:E427"/>
+    <mergeCell ref="G427:H427"/>
+    <mergeCell ref="A433:B433"/>
+    <mergeCell ref="D433:E433"/>
+    <mergeCell ref="G433:H433"/>
+    <mergeCell ref="A436:B436"/>
+    <mergeCell ref="D436:E436"/>
+    <mergeCell ref="G436:H436"/>
+    <mergeCell ref="A415:B415"/>
+    <mergeCell ref="D415:E415"/>
+    <mergeCell ref="G415:H415"/>
+    <mergeCell ref="A418:B418"/>
+    <mergeCell ref="D418:E418"/>
+    <mergeCell ref="G418:H418"/>
+    <mergeCell ref="A424:B424"/>
+    <mergeCell ref="D424:E424"/>
+    <mergeCell ref="G424:H424"/>
+    <mergeCell ref="A400:B400"/>
+    <mergeCell ref="D400:E400"/>
+    <mergeCell ref="G400:H400"/>
+    <mergeCell ref="A406:B406"/>
+    <mergeCell ref="D406:E406"/>
+    <mergeCell ref="G406:H406"/>
+    <mergeCell ref="A409:B409"/>
+    <mergeCell ref="D409:E409"/>
+    <mergeCell ref="G409:H409"/>
+    <mergeCell ref="A388:B388"/>
+    <mergeCell ref="D388:E388"/>
+    <mergeCell ref="G388:H388"/>
+    <mergeCell ref="A391:B391"/>
+    <mergeCell ref="D391:E391"/>
+    <mergeCell ref="G391:H391"/>
+    <mergeCell ref="A397:B397"/>
+    <mergeCell ref="D397:E397"/>
+    <mergeCell ref="G397:H397"/>
+    <mergeCell ref="A373:B373"/>
+    <mergeCell ref="D373:E373"/>
+    <mergeCell ref="G373:H373"/>
+    <mergeCell ref="A379:B379"/>
+    <mergeCell ref="D379:E379"/>
+    <mergeCell ref="G379:H379"/>
+    <mergeCell ref="A382:B382"/>
+    <mergeCell ref="D382:E382"/>
+    <mergeCell ref="G382:H382"/>
+    <mergeCell ref="A361:B361"/>
+    <mergeCell ref="D361:E361"/>
+    <mergeCell ref="G361:H361"/>
+    <mergeCell ref="A364:B364"/>
+    <mergeCell ref="D364:E364"/>
+    <mergeCell ref="G364:H364"/>
+    <mergeCell ref="A370:B370"/>
+    <mergeCell ref="D370:E370"/>
+    <mergeCell ref="G370:H370"/>
+    <mergeCell ref="A346:B346"/>
+    <mergeCell ref="D346:E346"/>
+    <mergeCell ref="G346:H346"/>
+    <mergeCell ref="A352:B352"/>
+    <mergeCell ref="D352:E352"/>
+    <mergeCell ref="G352:H352"/>
+    <mergeCell ref="A355:B355"/>
+    <mergeCell ref="D355:E355"/>
+    <mergeCell ref="G355:H355"/>
+    <mergeCell ref="A334:B334"/>
+    <mergeCell ref="D334:E334"/>
+    <mergeCell ref="G334:H334"/>
+    <mergeCell ref="A337:B337"/>
+    <mergeCell ref="D337:E337"/>
+    <mergeCell ref="G337:H337"/>
+    <mergeCell ref="A343:B343"/>
+    <mergeCell ref="D343:E343"/>
+    <mergeCell ref="G343:H343"/>
+    <mergeCell ref="A319:B319"/>
+    <mergeCell ref="D319:E319"/>
+    <mergeCell ref="G319:H319"/>
+    <mergeCell ref="A325:B325"/>
+    <mergeCell ref="D325:E325"/>
+    <mergeCell ref="G325:H325"/>
+    <mergeCell ref="A328:B328"/>
+    <mergeCell ref="D328:E328"/>
+    <mergeCell ref="G328:H328"/>
+    <mergeCell ref="A307:B307"/>
+    <mergeCell ref="D307:E307"/>
+    <mergeCell ref="G307:H307"/>
+    <mergeCell ref="A310:B310"/>
+    <mergeCell ref="D310:E310"/>
+    <mergeCell ref="G310:H310"/>
+    <mergeCell ref="A316:B316"/>
+    <mergeCell ref="D316:E316"/>
+    <mergeCell ref="G316:H316"/>
+    <mergeCell ref="A292:B292"/>
+    <mergeCell ref="D292:E292"/>
+    <mergeCell ref="G292:H292"/>
+    <mergeCell ref="A298:B298"/>
+    <mergeCell ref="D298:E298"/>
+    <mergeCell ref="G298:H298"/>
+    <mergeCell ref="A301:B301"/>
+    <mergeCell ref="D301:E301"/>
+    <mergeCell ref="G301:H301"/>
+    <mergeCell ref="D229:E229"/>
+    <mergeCell ref="G229:H229"/>
+    <mergeCell ref="A220:B220"/>
+    <mergeCell ref="D220:E220"/>
+    <mergeCell ref="G220:H220"/>
+    <mergeCell ref="A226:B226"/>
+    <mergeCell ref="D226:E226"/>
+    <mergeCell ref="G226:H226"/>
+    <mergeCell ref="A229:B229"/>
+    <mergeCell ref="D217:E217"/>
+    <mergeCell ref="G217:H217"/>
+    <mergeCell ref="A208:B208"/>
+    <mergeCell ref="D208:E208"/>
+    <mergeCell ref="G208:H208"/>
+    <mergeCell ref="A211:B211"/>
+    <mergeCell ref="D211:E211"/>
+    <mergeCell ref="G211:H211"/>
+    <mergeCell ref="A217:B217"/>
+    <mergeCell ref="D202:E202"/>
+    <mergeCell ref="G202:H202"/>
+    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="D193:E193"/>
+    <mergeCell ref="G193:H193"/>
+    <mergeCell ref="A199:B199"/>
+    <mergeCell ref="D199:E199"/>
+    <mergeCell ref="G199:H199"/>
+    <mergeCell ref="A202:B202"/>
+    <mergeCell ref="D166:E166"/>
+    <mergeCell ref="G166:H166"/>
+    <mergeCell ref="A172:B172"/>
+    <mergeCell ref="D172:E172"/>
+    <mergeCell ref="G172:H172"/>
+    <mergeCell ref="A175:B175"/>
+    <mergeCell ref="D190:E190"/>
+    <mergeCell ref="G190:H190"/>
+    <mergeCell ref="A181:B181"/>
+    <mergeCell ref="D181:E181"/>
+    <mergeCell ref="G181:H181"/>
+    <mergeCell ref="A184:B184"/>
+    <mergeCell ref="D184:E184"/>
+    <mergeCell ref="G184:H184"/>
+    <mergeCell ref="A190:B190"/>
     <mergeCell ref="A289:B289"/>
     <mergeCell ref="D289:E289"/>
     <mergeCell ref="G289:H289"/>
@@ -22635,324 +22835,132 @@
     <mergeCell ref="D175:E175"/>
     <mergeCell ref="G175:H175"/>
     <mergeCell ref="A166:B166"/>
-    <mergeCell ref="D166:E166"/>
-    <mergeCell ref="G166:H166"/>
-    <mergeCell ref="A172:B172"/>
-    <mergeCell ref="D172:E172"/>
-    <mergeCell ref="G172:H172"/>
-    <mergeCell ref="A175:B175"/>
-    <mergeCell ref="D190:E190"/>
-    <mergeCell ref="G190:H190"/>
-    <mergeCell ref="A181:B181"/>
-    <mergeCell ref="D181:E181"/>
-    <mergeCell ref="G181:H181"/>
-    <mergeCell ref="A184:B184"/>
-    <mergeCell ref="D184:E184"/>
-    <mergeCell ref="G184:H184"/>
-    <mergeCell ref="A190:B190"/>
-    <mergeCell ref="D202:E202"/>
-    <mergeCell ref="G202:H202"/>
-    <mergeCell ref="A193:B193"/>
-    <mergeCell ref="D193:E193"/>
-    <mergeCell ref="G193:H193"/>
-    <mergeCell ref="A199:B199"/>
-    <mergeCell ref="D199:E199"/>
-    <mergeCell ref="G199:H199"/>
-    <mergeCell ref="A202:B202"/>
-    <mergeCell ref="D217:E217"/>
-    <mergeCell ref="G217:H217"/>
-    <mergeCell ref="A208:B208"/>
-    <mergeCell ref="D208:E208"/>
-    <mergeCell ref="G208:H208"/>
-    <mergeCell ref="A211:B211"/>
-    <mergeCell ref="D211:E211"/>
-    <mergeCell ref="G211:H211"/>
-    <mergeCell ref="A217:B217"/>
-    <mergeCell ref="D229:E229"/>
-    <mergeCell ref="G229:H229"/>
-    <mergeCell ref="A220:B220"/>
-    <mergeCell ref="D220:E220"/>
-    <mergeCell ref="G220:H220"/>
-    <mergeCell ref="A226:B226"/>
-    <mergeCell ref="D226:E226"/>
-    <mergeCell ref="G226:H226"/>
-    <mergeCell ref="A229:B229"/>
-    <mergeCell ref="A292:B292"/>
-    <mergeCell ref="D292:E292"/>
-    <mergeCell ref="G292:H292"/>
-    <mergeCell ref="A298:B298"/>
-    <mergeCell ref="D298:E298"/>
-    <mergeCell ref="G298:H298"/>
-    <mergeCell ref="A301:B301"/>
-    <mergeCell ref="D301:E301"/>
-    <mergeCell ref="G301:H301"/>
-    <mergeCell ref="A307:B307"/>
-    <mergeCell ref="D307:E307"/>
-    <mergeCell ref="G307:H307"/>
-    <mergeCell ref="A310:B310"/>
-    <mergeCell ref="D310:E310"/>
-    <mergeCell ref="G310:H310"/>
-    <mergeCell ref="A316:B316"/>
-    <mergeCell ref="D316:E316"/>
-    <mergeCell ref="G316:H316"/>
-    <mergeCell ref="A319:B319"/>
-    <mergeCell ref="D319:E319"/>
-    <mergeCell ref="G319:H319"/>
-    <mergeCell ref="A325:B325"/>
-    <mergeCell ref="D325:E325"/>
-    <mergeCell ref="G325:H325"/>
-    <mergeCell ref="A328:B328"/>
-    <mergeCell ref="D328:E328"/>
-    <mergeCell ref="G328:H328"/>
-    <mergeCell ref="A334:B334"/>
-    <mergeCell ref="D334:E334"/>
-    <mergeCell ref="G334:H334"/>
-    <mergeCell ref="A337:B337"/>
-    <mergeCell ref="D337:E337"/>
-    <mergeCell ref="G337:H337"/>
-    <mergeCell ref="A343:B343"/>
-    <mergeCell ref="D343:E343"/>
-    <mergeCell ref="G343:H343"/>
-    <mergeCell ref="A346:B346"/>
-    <mergeCell ref="D346:E346"/>
-    <mergeCell ref="G346:H346"/>
-    <mergeCell ref="A352:B352"/>
-    <mergeCell ref="D352:E352"/>
-    <mergeCell ref="G352:H352"/>
-    <mergeCell ref="A355:B355"/>
-    <mergeCell ref="D355:E355"/>
-    <mergeCell ref="G355:H355"/>
-    <mergeCell ref="A361:B361"/>
-    <mergeCell ref="D361:E361"/>
-    <mergeCell ref="G361:H361"/>
-    <mergeCell ref="A364:B364"/>
-    <mergeCell ref="D364:E364"/>
-    <mergeCell ref="G364:H364"/>
-    <mergeCell ref="A370:B370"/>
-    <mergeCell ref="D370:E370"/>
-    <mergeCell ref="G370:H370"/>
-    <mergeCell ref="A373:B373"/>
-    <mergeCell ref="D373:E373"/>
-    <mergeCell ref="G373:H373"/>
-    <mergeCell ref="A379:B379"/>
-    <mergeCell ref="D379:E379"/>
-    <mergeCell ref="G379:H379"/>
-    <mergeCell ref="A382:B382"/>
-    <mergeCell ref="D382:E382"/>
-    <mergeCell ref="G382:H382"/>
-    <mergeCell ref="A388:B388"/>
-    <mergeCell ref="D388:E388"/>
-    <mergeCell ref="G388:H388"/>
-    <mergeCell ref="A391:B391"/>
-    <mergeCell ref="D391:E391"/>
-    <mergeCell ref="G391:H391"/>
-    <mergeCell ref="A397:B397"/>
-    <mergeCell ref="D397:E397"/>
-    <mergeCell ref="G397:H397"/>
-    <mergeCell ref="A400:B400"/>
-    <mergeCell ref="D400:E400"/>
-    <mergeCell ref="G400:H400"/>
-    <mergeCell ref="A406:B406"/>
-    <mergeCell ref="D406:E406"/>
-    <mergeCell ref="G406:H406"/>
-    <mergeCell ref="A409:B409"/>
-    <mergeCell ref="D409:E409"/>
-    <mergeCell ref="G409:H409"/>
-    <mergeCell ref="A415:B415"/>
-    <mergeCell ref="D415:E415"/>
-    <mergeCell ref="G415:H415"/>
-    <mergeCell ref="A418:B418"/>
-    <mergeCell ref="D418:E418"/>
-    <mergeCell ref="G418:H418"/>
-    <mergeCell ref="A424:B424"/>
-    <mergeCell ref="D424:E424"/>
-    <mergeCell ref="G424:H424"/>
-    <mergeCell ref="A427:B427"/>
-    <mergeCell ref="D427:E427"/>
-    <mergeCell ref="G427:H427"/>
-    <mergeCell ref="A433:B433"/>
-    <mergeCell ref="D433:E433"/>
-    <mergeCell ref="G433:H433"/>
-    <mergeCell ref="A436:B436"/>
-    <mergeCell ref="D436:E436"/>
-    <mergeCell ref="G436:H436"/>
-    <mergeCell ref="A442:B442"/>
-    <mergeCell ref="D442:E442"/>
-    <mergeCell ref="G442:H442"/>
-    <mergeCell ref="A445:B445"/>
-    <mergeCell ref="D445:E445"/>
-    <mergeCell ref="G445:H445"/>
-    <mergeCell ref="A451:B451"/>
-    <mergeCell ref="D451:E451"/>
-    <mergeCell ref="G451:H451"/>
-    <mergeCell ref="A463:B463"/>
-    <mergeCell ref="D463:E463"/>
-    <mergeCell ref="G463:H463"/>
-    <mergeCell ref="A469:B469"/>
-    <mergeCell ref="D469:E469"/>
-    <mergeCell ref="G469:H469"/>
-    <mergeCell ref="A454:B454"/>
-    <mergeCell ref="D454:E454"/>
-    <mergeCell ref="G454:H454"/>
-    <mergeCell ref="A460:B460"/>
-    <mergeCell ref="D460:E460"/>
-    <mergeCell ref="G460:H460"/>
-    <mergeCell ref="A472:B472"/>
-    <mergeCell ref="D472:E472"/>
-    <mergeCell ref="G472:H472"/>
-    <mergeCell ref="A478:B478"/>
-    <mergeCell ref="D478:E478"/>
-    <mergeCell ref="G478:H478"/>
-    <mergeCell ref="A481:B481"/>
-    <mergeCell ref="D481:E481"/>
-    <mergeCell ref="G481:H481"/>
-    <mergeCell ref="A487:B487"/>
-    <mergeCell ref="D487:E487"/>
-    <mergeCell ref="G487:H487"/>
-    <mergeCell ref="A490:B490"/>
-    <mergeCell ref="D490:E490"/>
-    <mergeCell ref="G490:H490"/>
-    <mergeCell ref="A496:B496"/>
-    <mergeCell ref="D496:E496"/>
-    <mergeCell ref="G496:H496"/>
-    <mergeCell ref="A499:B499"/>
-    <mergeCell ref="D499:E499"/>
-    <mergeCell ref="G499:H499"/>
-    <mergeCell ref="A505:B505"/>
-    <mergeCell ref="D505:E505"/>
-    <mergeCell ref="G505:H505"/>
-    <mergeCell ref="A508:B508"/>
-    <mergeCell ref="D508:E508"/>
-    <mergeCell ref="G508:H508"/>
-    <mergeCell ref="A514:B514"/>
-    <mergeCell ref="D514:E514"/>
-    <mergeCell ref="G514:H514"/>
-    <mergeCell ref="A517:B517"/>
-    <mergeCell ref="D517:E517"/>
-    <mergeCell ref="G517:H517"/>
-    <mergeCell ref="A523:B523"/>
-    <mergeCell ref="D523:E523"/>
-    <mergeCell ref="G523:H523"/>
-    <mergeCell ref="A526:B526"/>
-    <mergeCell ref="D526:E526"/>
-    <mergeCell ref="G526:H526"/>
-    <mergeCell ref="A532:B532"/>
-    <mergeCell ref="D532:E532"/>
-    <mergeCell ref="G532:H532"/>
-    <mergeCell ref="A535:B535"/>
-    <mergeCell ref="D535:E535"/>
-    <mergeCell ref="G535:H535"/>
-    <mergeCell ref="A541:B541"/>
-    <mergeCell ref="D541:E541"/>
-    <mergeCell ref="G541:H541"/>
-    <mergeCell ref="A544:B544"/>
-    <mergeCell ref="D544:E544"/>
-    <mergeCell ref="G544:H544"/>
-    <mergeCell ref="A550:B550"/>
-    <mergeCell ref="D550:E550"/>
-    <mergeCell ref="G550:H550"/>
-    <mergeCell ref="A553:B553"/>
-    <mergeCell ref="D553:E553"/>
-    <mergeCell ref="G553:H553"/>
-    <mergeCell ref="A559:B559"/>
-    <mergeCell ref="D559:E559"/>
-    <mergeCell ref="G559:H559"/>
-    <mergeCell ref="A562:B562"/>
-    <mergeCell ref="D562:E562"/>
-    <mergeCell ref="G562:H562"/>
-    <mergeCell ref="A568:B568"/>
-    <mergeCell ref="D568:E568"/>
-    <mergeCell ref="G568:H568"/>
-    <mergeCell ref="A571:B571"/>
-    <mergeCell ref="D571:E571"/>
-    <mergeCell ref="G571:H571"/>
-    <mergeCell ref="A577:B577"/>
-    <mergeCell ref="D577:E577"/>
-    <mergeCell ref="G577:H577"/>
-    <mergeCell ref="A580:B580"/>
-    <mergeCell ref="D580:E580"/>
-    <mergeCell ref="G580:H580"/>
-    <mergeCell ref="A586:B586"/>
-    <mergeCell ref="D586:E586"/>
-    <mergeCell ref="G586:H586"/>
-    <mergeCell ref="A589:B589"/>
-    <mergeCell ref="D589:E589"/>
-    <mergeCell ref="G589:H589"/>
-    <mergeCell ref="A595:B595"/>
-    <mergeCell ref="D595:E595"/>
-    <mergeCell ref="G595:H595"/>
-    <mergeCell ref="A598:B598"/>
-    <mergeCell ref="D598:E598"/>
-    <mergeCell ref="G598:H598"/>
-    <mergeCell ref="A604:B604"/>
-    <mergeCell ref="D604:E604"/>
-    <mergeCell ref="G604:H604"/>
-    <mergeCell ref="A607:B607"/>
-    <mergeCell ref="D607:E607"/>
-    <mergeCell ref="G607:H607"/>
-    <mergeCell ref="A613:B613"/>
-    <mergeCell ref="D613:E613"/>
-    <mergeCell ref="G613:H613"/>
-    <mergeCell ref="A616:B616"/>
-    <mergeCell ref="D616:E616"/>
-    <mergeCell ref="G616:H616"/>
-    <mergeCell ref="A622:B622"/>
-    <mergeCell ref="D622:E622"/>
-    <mergeCell ref="G622:H622"/>
-    <mergeCell ref="A625:B625"/>
-    <mergeCell ref="D625:E625"/>
-    <mergeCell ref="G625:H625"/>
-    <mergeCell ref="A631:B631"/>
-    <mergeCell ref="D631:E631"/>
-    <mergeCell ref="G631:H631"/>
-    <mergeCell ref="A634:B634"/>
-    <mergeCell ref="D634:E634"/>
-    <mergeCell ref="G634:H634"/>
-    <mergeCell ref="A640:B640"/>
-    <mergeCell ref="D640:E640"/>
-    <mergeCell ref="G640:H640"/>
-    <mergeCell ref="A643:B643"/>
-    <mergeCell ref="D643:E643"/>
-    <mergeCell ref="G643:H643"/>
-    <mergeCell ref="A649:B649"/>
-    <mergeCell ref="D649:E649"/>
-    <mergeCell ref="G649:H649"/>
-    <mergeCell ref="A652:B652"/>
-    <mergeCell ref="D652:E652"/>
-    <mergeCell ref="G652:H652"/>
-    <mergeCell ref="A658:B658"/>
-    <mergeCell ref="D658:E658"/>
-    <mergeCell ref="G658:H658"/>
-    <mergeCell ref="A661:B661"/>
-    <mergeCell ref="D661:E661"/>
-    <mergeCell ref="G661:H661"/>
-    <mergeCell ref="A667:B667"/>
-    <mergeCell ref="D667:E667"/>
-    <mergeCell ref="G667:H667"/>
-    <mergeCell ref="A670:B670"/>
-    <mergeCell ref="D670:E670"/>
-    <mergeCell ref="G670:H670"/>
-    <mergeCell ref="A676:B676"/>
-    <mergeCell ref="D676:E676"/>
-    <mergeCell ref="G676:H676"/>
-    <mergeCell ref="A679:B679"/>
-    <mergeCell ref="D679:E679"/>
-    <mergeCell ref="G679:H679"/>
-    <mergeCell ref="A685:B685"/>
-    <mergeCell ref="D685:E685"/>
-    <mergeCell ref="G685:H685"/>
-    <mergeCell ref="A703:B703"/>
-    <mergeCell ref="D703:E703"/>
-    <mergeCell ref="G703:H703"/>
-    <mergeCell ref="A688:B688"/>
-    <mergeCell ref="D688:E688"/>
-    <mergeCell ref="G688:H688"/>
-    <mergeCell ref="A694:B694"/>
-    <mergeCell ref="D694:E694"/>
-    <mergeCell ref="G694:H694"/>
-    <mergeCell ref="A697:B697"/>
-    <mergeCell ref="D697:E697"/>
-    <mergeCell ref="G697:H697"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D283:E283"/>
+    <mergeCell ref="G283:H283"/>
+    <mergeCell ref="A274:B274"/>
+    <mergeCell ref="D274:E274"/>
+    <mergeCell ref="G274:H274"/>
+    <mergeCell ref="A280:B280"/>
+    <mergeCell ref="D280:E280"/>
+    <mergeCell ref="G280:H280"/>
+    <mergeCell ref="A283:B283"/>
+    <mergeCell ref="D271:E271"/>
+    <mergeCell ref="G271:H271"/>
+    <mergeCell ref="A262:B262"/>
+    <mergeCell ref="D262:E262"/>
+    <mergeCell ref="G262:H262"/>
+    <mergeCell ref="A265:B265"/>
+    <mergeCell ref="D265:E265"/>
+    <mergeCell ref="G265:H265"/>
+    <mergeCell ref="A271:B271"/>
+    <mergeCell ref="D256:E256"/>
+    <mergeCell ref="G256:H256"/>
+    <mergeCell ref="A247:B247"/>
+    <mergeCell ref="D247:E247"/>
+    <mergeCell ref="G247:H247"/>
+    <mergeCell ref="A253:B253"/>
+    <mergeCell ref="D253:E253"/>
+    <mergeCell ref="G253:H253"/>
+    <mergeCell ref="A256:B256"/>
+    <mergeCell ref="D244:E244"/>
+    <mergeCell ref="G244:H244"/>
+    <mergeCell ref="A235:B235"/>
+    <mergeCell ref="D235:E235"/>
+    <mergeCell ref="G235:H235"/>
+    <mergeCell ref="A238:B238"/>
+    <mergeCell ref="D238:E238"/>
+    <mergeCell ref="G238:H238"/>
+    <mergeCell ref="A244:B244"/>
+    <mergeCell ref="D136:E136"/>
+    <mergeCell ref="G136:H136"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="D127:E127"/>
+    <mergeCell ref="G127:H127"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="G130:H130"/>
+    <mergeCell ref="A136:B136"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="G121:H121"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="G112:H112"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="D118:E118"/>
+    <mergeCell ref="G118:H118"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="G109:H109"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="G100:H100"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="G103:H103"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="G94:H94"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="G85:H85"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="G91:H91"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="G82:H82"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="G76:H76"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="G64:H64"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="A55:B55"/>
   </mergeCells>
   <pageMargins left="0.17" right="0.19" top="0.21" bottom="0.18" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>